<commit_message>
redid template w/ updated civilian_complaints tab name
</commit_message>
<xml_diff>
--- a/publisher/public/assets/LAW_ENFORCEMENT.xlsx
+++ b/publisher/public/assets/LAW_ENFORCEMENT.xlsx
@@ -25,8 +25,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="arrests_by_biological_sex" sheetId="16" state="visible" r:id="rId16"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="use_of_force" sheetId="17" state="visible" r:id="rId17"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="use_of_force_by_type" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="civilian_complaints_sustained" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="civilian_complaints_sustained_by_type" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="civilian_complaints" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="civilian_complaints_by_type" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>